<commit_message>
contagem de portarias fixada
</commit_message>
<xml_diff>
--- a/tabelas/processos_siout_2021-02-08.xlsx
+++ b/tabelas/processos_siout_2021-02-08.xlsx
@@ -675,7 +675,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -685,12 +685,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>18/01/2021</t>
+          <t>08/02/2021</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.028/2021</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.029/2021</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.030/2021</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.031/2021</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.032/2021</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1309,12 +1309,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>29/10/2020</t>
+          <t>08/02/2021</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.033/2021</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1361,12 +1361,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>29/10/2020</t>
+          <t>08/02/2021</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.034/2021</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.035/2021</t>
         </is>
       </c>
     </row>
@@ -3535,7 +3535,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3545,12 +3545,12 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>21/01/2021</t>
+          <t>08/02/2021</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.036/2021</t>
         </is>
       </c>
     </row>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Em análise</t>
+          <t>Concedida</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>000.037/2021</t>
         </is>
       </c>
     </row>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Aguardando alterações de dados inconsistentes</t>
+          <t>Aguardando análise</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">

</xml_diff>